<commit_message>
Update readmes & example file
Renaming hierarchy_as_indent ->hierarchy_to_indent
to avoid confusion about direction of conversion.
</commit_message>
<xml_diff>
--- a/example/indent_3spaces_043_4Cat.xlsx
+++ b/example/indent_3spaces_043_4Cat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="28830" windowHeight="14490" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="105">
   <si>
     <t xml:space="preserve">Created by </t>
   </si>
@@ -824,14 +824,20 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -842,12 +848,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1302,7 +1302,7 @@
       <c r="E2" s="36"/>
       <c r="F2" s="36"/>
       <c r="G2" s="36"/>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="47" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="48"/>
@@ -1369,7 +1369,7 @@
       <c r="E7" s="36"/>
       <c r="F7" s="36"/>
       <c r="G7" s="36"/>
-      <c r="H7" s="49" t="s">
+      <c r="H7" s="47" t="s">
         <v>1</v>
       </c>
       <c r="I7" s="48"/>
@@ -1384,7 +1384,7 @@
       <c r="E8" s="36"/>
       <c r="F8" s="36"/>
       <c r="G8" s="36"/>
-      <c r="H8" s="55" t="s">
+      <c r="H8" s="50" t="s">
         <v>2</v>
       </c>
       <c r="I8" s="48"/>
@@ -1399,7 +1399,7 @@
       <c r="E9" s="36"/>
       <c r="F9" s="36"/>
       <c r="G9" s="36"/>
-      <c r="H9" s="50"/>
+      <c r="H9" s="51"/>
       <c r="I9" s="48"/>
       <c r="J9" s="48"/>
       <c r="K9" s="36"/>
@@ -1412,7 +1412,7 @@
       <c r="E10" s="36"/>
       <c r="F10" s="36"/>
       <c r="G10" s="36"/>
-      <c r="H10" s="50" t="s">
+      <c r="H10" s="51" t="s">
         <v>3</v>
       </c>
       <c r="I10" s="48"/>
@@ -1457,7 +1457,7 @@
       <c r="E13" s="36"/>
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
-      <c r="H13" s="51" t="s">
+      <c r="H13" s="53" t="s">
         <v>6</v>
       </c>
       <c r="I13" s="48"/>
@@ -1472,7 +1472,7 @@
       <c r="E14" s="36"/>
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
-      <c r="H14" s="50" t="s">
+      <c r="H14" s="51" t="s">
         <v>7</v>
       </c>
       <c r="I14" s="48"/>
@@ -1493,11 +1493,11 @@
       <c r="K15" s="36"/>
     </row>
     <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="54" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="48"/>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="55" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="48"/>
@@ -1510,11 +1510,11 @@
       <c r="K16" s="36"/>
     </row>
     <row r="17" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="54" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="48"/>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="49" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="48"/>
@@ -1540,7 +1540,7 @@
       <c r="K18" s="36"/>
     </row>
     <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="52" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="48"/>
@@ -1594,7 +1594,7 @@
       <c r="K22" s="36"/>
     </row>
     <row r="23" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="50" t="s">
+      <c r="A23" s="51" t="s">
         <v>13</v>
       </c>
       <c r="B23" s="48"/>
@@ -1622,7 +1622,7 @@
       <c r="K24" s="36"/>
     </row>
     <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="47" t="s">
+      <c r="A25" s="52" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="48"/>
@@ -1650,7 +1650,7 @@
       <c r="K26" s="36"/>
     </row>
     <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="47" t="s">
+      <c r="A27" s="52" t="s">
         <v>15</v>
       </c>
       <c r="B27" s="48"/>
@@ -2656,11 +2656,6 @@
     <row r="1005" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="A25:G25"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="H10:J10"/>
@@ -2671,6 +2666,11 @@
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="A25:G25"/>
   </mergeCells>
   <conditionalFormatting sqref="H17:J18 K1:K8 K17:K28 H3:J7 H10:J10 H8 K10:K15 H13:J13 H14 A18:G18 A15:J15 A19:J28 A10:G14 A2:G8 A1:J1 A9:K9">
     <cfRule type="containsBlanks" dxfId="9" priority="13">
@@ -8761,7 +8761,7 @@
   <dimension ref="A1:J546"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G11"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8839,9 +8839,7 @@
       <c r="D3" s="45"/>
       <c r="E3" s="35"/>
       <c r="F3" s="45"/>
-      <c r="G3" s="43" t="s">
-        <v>69</v>
-      </c>
+      <c r="G3" s="43"/>
       <c r="H3" s="45"/>
       <c r="I3" s="45"/>
       <c r="J3" s="45"/>
@@ -8859,9 +8857,7 @@
       <c r="D4" s="35"/>
       <c r="E4" s="35"/>
       <c r="F4" s="45"/>
-      <c r="G4" s="43" t="s">
-        <v>69</v>
-      </c>
+      <c r="G4" s="43"/>
       <c r="H4" s="45"/>
       <c r="I4" s="45"/>
       <c r="J4" s="45"/>
@@ -8879,9 +8875,7 @@
       <c r="D5" s="45"/>
       <c r="E5" s="35"/>
       <c r="F5" s="45"/>
-      <c r="G5" s="43" t="s">
-        <v>69</v>
-      </c>
+      <c r="G5" s="43"/>
       <c r="H5" s="45"/>
       <c r="I5" s="45"/>
       <c r="J5" s="45"/>
@@ -8899,9 +8893,7 @@
       <c r="D6" s="45"/>
       <c r="E6" s="35"/>
       <c r="F6" s="45"/>
-      <c r="G6" s="43" t="s">
-        <v>69</v>
-      </c>
+      <c r="G6" s="43"/>
       <c r="H6" s="45"/>
       <c r="I6" s="45"/>
       <c r="J6" s="45"/>
@@ -8919,9 +8911,7 @@
       <c r="D7" s="45"/>
       <c r="E7" s="35"/>
       <c r="F7" s="45"/>
-      <c r="G7" s="43" t="s">
-        <v>69</v>
-      </c>
+      <c r="G7" s="43"/>
       <c r="H7" s="45"/>
       <c r="I7" s="45"/>
       <c r="J7" s="45"/>
@@ -8939,9 +8929,7 @@
       <c r="D8" s="45"/>
       <c r="E8" s="35"/>
       <c r="F8" s="45"/>
-      <c r="G8" s="43" t="s">
-        <v>69</v>
-      </c>
+      <c r="G8" s="43"/>
       <c r="H8" s="45"/>
       <c r="I8" s="45"/>
       <c r="J8" s="45"/>
@@ -8959,9 +8947,7 @@
       <c r="D9" s="45"/>
       <c r="E9" s="35"/>
       <c r="F9" s="45"/>
-      <c r="G9" s="43" t="s">
-        <v>69</v>
-      </c>
+      <c r="G9" s="43"/>
       <c r="H9" s="45"/>
       <c r="I9" s="45"/>
       <c r="J9" s="45"/>
@@ -8979,9 +8965,7 @@
       <c r="D10" s="45"/>
       <c r="E10" s="35"/>
       <c r="F10" s="45"/>
-      <c r="G10" s="43" t="s">
-        <v>69</v>
-      </c>
+      <c r="G10" s="43"/>
       <c r="H10" s="45"/>
       <c r="I10" s="45"/>
       <c r="J10" s="45"/>
@@ -8999,9 +8983,7 @@
       <c r="D11" s="45"/>
       <c r="E11" s="35"/>
       <c r="F11" s="45"/>
-      <c r="G11" s="43" t="s">
-        <v>69</v>
-      </c>
+      <c r="G11" s="43"/>
       <c r="H11" s="45"/>
       <c r="I11" s="45"/>
       <c r="J11" s="45"/>

</xml_diff>